<commit_message>
added image links to color family list
</commit_message>
<xml_diff>
--- a/gothicTextsDb.xlsx
+++ b/gothicTextsDb.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8000" windowHeight="14740" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Gothic Texts" sheetId="1" r:id="rId1"/>
     <sheet name="Colour Names" sheetId="2" r:id="rId2"/>
+    <sheet name="Colour Families" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Gothic Texts'!$A$1:$AA$412</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11076" uniqueCount="3219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11261" uniqueCount="3255">
   <si>
     <t>Title</t>
   </si>
@@ -9694,6 +9695,114 @@
   </si>
   <si>
     <t>Who's The Murderer? Or, The Mystery Of The Forest</t>
+  </si>
+  <si>
+    <t>Colour Famiily</t>
+  </si>
+  <si>
+    <t>Link to Image</t>
+  </si>
+  <si>
+    <t>http://www.ansiindia.com/blowups/pure-white-pebbles.jpg</t>
+  </si>
+  <si>
+    <t>http://www.marcodebiasi.net/MDhobbies/MDphoto/photogalleries/nature/whitesnow05.jpg</t>
+  </si>
+  <si>
+    <t>http://cdn1.medicalnewstoday.com/content/images/articles/273451-milk.jpg</t>
+  </si>
+  <si>
+    <t>http://i.ebayimg.com/00/s/MzQ4WDM0OA==/z/DBAAAOSwZVlXnmGm/$_1.JPG?set_id=2</t>
+  </si>
+  <si>
+    <t>https://tse1.mm.bing.net/th?id=OIP.YoTvnt8BqgxkpLIDaOfXCgEsC7&amp;pid=Api&amp;w=288&amp;h=181</t>
+  </si>
+  <si>
+    <t>https://img1.etsystatic.com/115/0/13166338/il_570xN.1034939389_3avz.jpg</t>
+  </si>
+  <si>
+    <t>https://s-media-cache-ak0.pinimg.com/originals/0a/a7/86/0aa78698cf792ae00aa9820469627480.jpg</t>
+  </si>
+  <si>
+    <t>http://www.inneocreative.com/wp-content/uploads/2011/11/alabaster-bianco-32x64.jpg</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn3.gstatic.com/images?q=tbn:ANd9GcRNHMTsW08tA6iW262oVeKsdPOYcTMoD23e-8rSbpx-jomr_z-4</t>
+  </si>
+  <si>
+    <t>https://3.imimg.com/data3/HT/BS/MY-3476148/raw-cotton-250x250.jpg</t>
+  </si>
+  <si>
+    <t>http://www.lifetasteslikefood.com/wp-content/uploads/2012/01/IMG_8891-1024x682.jpg</t>
+  </si>
+  <si>
+    <t>http://upload.wikimedia.org/wikipedia/commons/thumb/2/27/Sample_of_jet_2013.JPG/300px-Sample_of_jet_2013.JPG</t>
+  </si>
+  <si>
+    <t>http://energynewsbd.com/panel/newspicture/1465400395c.jpg</t>
+  </si>
+  <si>
+    <t>http://www.qingdaonese.com/wp-content/uploads/2012/04/qingdaophotos_nightskyHuangdao.jpg</t>
+  </si>
+  <si>
+    <t>http://wpmedia.edmontonjournal.com/2016/02/edmonton-alberta-july-6-2015-a-raven-perchs-on-a-trash-c.jpeg?quality=55&amp;strip=all&amp;w=840&amp;h=630&amp;crop=1</t>
+  </si>
+  <si>
+    <t>http://www.bluemaize.net/im/arts-crafts-sewing/black-ink-9.jpg</t>
+  </si>
+  <si>
+    <t>https://i.kinja-img.com/gawker-media/image/upload/t_original/685722504901980592.jpg</t>
+  </si>
+  <si>
+    <t>https://us.123rf.com/450wm/kzwwsko/kzwwsko1503/kzwwsko150302309/37644600-black-soot-on-the-metal.jpg?ver=6</t>
+  </si>
+  <si>
+    <t>http://www.shzongyue.com/data/out/102/39584753-rose-red.jpg</t>
+  </si>
+  <si>
+    <t>http://wonderopolis.org/wp-content/uploads//2014/03/dreamstime_xl_13459006-custom.jpg</t>
+  </si>
+  <si>
+    <t>http://www.churchofthemessiah.ca/wp-content/uploads/2014/10/29987836_xl-200x300.jpg</t>
+  </si>
+  <si>
+    <t>https://www.bbcgoodfood.com/sites/default/files/glossary/avocado.jpg</t>
+  </si>
+  <si>
+    <t>http://fox41blogs.typepad.com/.a/6a0148c78b79ee970c017d411f6990970c-500wi</t>
+  </si>
+  <si>
+    <t>https://static1.squarespace.com/static/538d3109e4b0f6391fd9ca16/t/539a43b7e4b0c09f2ad2c586/1402618868669/SeaIslandIndigo_workshops2.jpg?format=1500w</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/7/6197/6127537096_630787a494_b.jpg</t>
+  </si>
+  <si>
+    <t>https://us.123rf.com/450wm/phittavas/phittavas1412/phittavas141200093/34350029-fly-ash-raw-material-for-mix-with-concrete-as-background.jpg?ver=6</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/7/79/FEMA_-_33369_-_Fire_and_smoke_in_California_as_helicopters_drop_water.jpg/800px-FEMA_-_33369_-_Fire_and_smoke_in_California_as_helicopters_drop_water.jpg</t>
+  </si>
+  <si>
+    <t>http://www.hannibalservices.com/productos/minerales.jpg</t>
+  </si>
+  <si>
+    <t>http://www.gravitatechnomech.com/images/Lead.jpg</t>
+  </si>
+  <si>
+    <t>http://vgawesomerocks.weebly.com/uploads/1/6/5/8/16581868/6837395.jpg</t>
+  </si>
+  <si>
+    <t>https://ae01.alicdn.com/kf/HTB1k_8qLFXXXXchXXXXq6xXFXXXs/5strand-lot-7-8mm-silver-font-b-grey-b-font-color-baroque-font-b-pearl-b.jpg</t>
+  </si>
+  <si>
+    <t>https://fthmb.tqn.com/-3Dpev8PKsTpjhn9v39uwhl2mxk=/768x0/filters:no_upscale()/about/GettyImages-121840901-56f0a1d73df78ce5f83b528a.jpg</t>
+  </si>
+  <si>
+    <t>https://s-media-cache-ak0.pinimg.com/236x/41/4b/ff/414bffdab3431f5c1167775d138809a1.jpg</t>
+  </si>
+  <si>
+    <t>http://www.chemicool.com/elements/images/300-galena.jpg</t>
   </si>
 </sst>
 </file>
@@ -10617,7 +10726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA412"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -59824,4 +59933,942 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B170"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>3219</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="17" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="17" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="17" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="17" t="s">
+        <v>410</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="17" t="s">
+        <v>411</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="17" t="s">
+        <v>412</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="17" t="s">
+        <v>413</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="17" t="s">
+        <v>414</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="17" t="s">
+        <v>415</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="17" t="s">
+        <v>416</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="17" t="s">
+        <v>418</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3229</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="17" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="17" t="s">
+        <v>419</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="17" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="17" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="17" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="17" t="s">
+        <v>424</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3254</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="17" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="17" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="17" t="s">
+        <v>440</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="17" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="17" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="17" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="17" t="s">
+        <v>468</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="17" t="s">
+        <v>474</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3233</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="17" t="s">
+        <v>478</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3234</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="17" t="s">
+        <v>481</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3235</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="17" t="s">
+        <v>487</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3236</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="17" t="s">
+        <v>496</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="17" t="s">
+        <v>503</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3238</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="17" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="17" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="17" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="17" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="17" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="17" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="17" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="17" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="17" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="17" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="17" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="17" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="17" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="17" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="17" t="s">
+        <v>697</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3239</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="17" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="17" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="17" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="17" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="17" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="17" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="17" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="17" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="17" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="17" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="17" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="17" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="17" t="s">
+        <v>847</v>
+      </c>
+      <c r="B60" t="s">
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="17" t="s">
+        <v>849</v>
+      </c>
+      <c r="B61" t="s">
+        <v>3241</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="17" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="17" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="17" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="17" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="17" t="s">
+        <v>888</v>
+      </c>
+      <c r="B66" t="s">
+        <v>3242</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="17" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="17" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="17" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="17" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="17" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="17" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="17" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="17" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="17" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="17" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="17" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="17" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="17" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="17" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="17" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="17" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="17" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="17" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="17" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="17" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="17" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="17" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="17" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="17" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="17" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="17" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B92" t="s">
+        <v>3243</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="17" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="17" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="17" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="17" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B96" t="s">
+        <v>3244</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="17" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="17" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="17" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="17" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="17" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="17" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="17" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="17" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="17" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="17" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="17" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="17" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="17" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="17" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="17" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="17" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="17" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="17" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B114" t="s">
+        <v>3245</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="17" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="17" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="17" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="17" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="17" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="17" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="17" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="17" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B122" t="s">
+        <v>3246</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="17" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B123" t="s">
+        <v>3247</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="17" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B124" t="s">
+        <v>3248</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="17" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B125" t="s">
+        <v>3249</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="17" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="17" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B127" t="s">
+        <v>3250</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="17" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B128" t="s">
+        <v>3251</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="17" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="17" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="17" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="17" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="17" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="17" t="s">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="17" t="s">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="17" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="17" t="s">
+        <v>1482</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="17" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" s="17" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" s="17" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" s="17" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" s="17" t="s">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" s="17" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" s="17" t="s">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" s="17" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="17" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" s="17" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="17" t="s">
+        <v>1543</v>
+      </c>
+      <c r="B148" t="s">
+        <v>3252</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="17" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="17" t="s">
+        <v>1548</v>
+      </c>
+      <c r="B150" t="s">
+        <v>3253</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" s="17"/>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" s="17"/>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" s="17"/>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" s="17"/>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" s="17"/>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" s="17"/>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" s="17"/>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" s="17"/>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" s="17"/>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" s="17"/>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" s="17"/>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" s="17"/>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" s="17"/>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" s="17"/>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" s="17"/>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" s="17"/>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" s="17"/>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" s="17"/>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" s="17"/>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>